<commit_message>
added trading opening module
</commit_message>
<xml_diff>
--- a/db/bin/real_trade_db_2024-09-18.xlsx
+++ b/db/bin/real_trade_db_2024-09-18.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z134"/>
+  <dimension ref="A1:Z152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12122,7 +12122,7 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B125" t="n">
         <v>2</v>
@@ -12214,7 +12214,7 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B126" t="n">
         <v>5</v>
@@ -12310,7 +12310,7 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127" t="n">
         <v>6</v>
@@ -12406,7 +12406,7 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128" t="n">
         <v>7</v>
@@ -12502,7 +12502,7 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129" t="n">
         <v>8</v>
@@ -12598,7 +12598,7 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B130" t="n">
         <v>10</v>
@@ -12694,7 +12694,7 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B131" t="n">
         <v>11</v>
@@ -12790,7 +12790,7 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B132" t="n">
         <v>12</v>
@@ -12882,7 +12882,7 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B133" t="n">
         <v>13</v>
@@ -12974,7 +12974,7 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B134" t="n">
         <v>15</v>
@@ -13063,6 +13063,1650 @@
         </is>
       </c>
       <c r="Z134" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="n">
+        <v>0</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>SYK</t>
+        </is>
+      </c>
+      <c r="D135" s="2" t="n">
+        <v>45553.19157438658</v>
+      </c>
+      <c r="E135" t="n">
+        <v>365.23</v>
+      </c>
+      <c r="F135" t="n">
+        <v>2191.38</v>
+      </c>
+      <c r="G135" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H135" s="2" t="n">
+        <v>45553.23894758102</v>
+      </c>
+      <c r="I135" t="n">
+        <v>365.295</v>
+      </c>
+      <c r="J135" t="n">
+        <v>2191.77</v>
+      </c>
+      <c r="K135" t="n">
+        <v>1.101</v>
+      </c>
+      <c r="L135" t="n">
+        <v>6</v>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N135" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O135" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P135" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q135" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R135" t="n">
+        <v>-0.7310000000001273</v>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>FA197B2DFEECC4A000</t>
+        </is>
+      </c>
+      <c r="T135" t="inlineStr"/>
+      <c r="U135" t="inlineStr">
+        <is>
+          <t>FA197B2E8EB504A000</t>
+        </is>
+      </c>
+      <c r="V135" t="inlineStr">
+        <is>
+          <t>FA197B2E8F0D04A000</t>
+        </is>
+      </c>
+      <c r="W135" t="inlineStr">
+        <is>
+          <t>FA197B2E2FB744A000</t>
+        </is>
+      </c>
+      <c r="X135" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y135" t="inlineStr">
+        <is>
+          <t>mv :-1.79, mv_2m:0.07,  mv_5m : 0.36, mv_30m : -2.46, mv_60m: 2.97</t>
+        </is>
+      </c>
+      <c r="Z135" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="n">
+        <v>1</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>SYK</t>
+        </is>
+      </c>
+      <c r="D136" s="2" t="n">
+        <v>45553.20124928241</v>
+      </c>
+      <c r="E136" t="n">
+        <v>364.9933</v>
+      </c>
+      <c r="F136" t="n">
+        <v>2189.9598</v>
+      </c>
+      <c r="G136" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H136" s="2" t="n">
+        <v>45553.24564335648</v>
+      </c>
+      <c r="I136" t="n">
+        <v>364.4441</v>
+      </c>
+      <c r="J136" t="n">
+        <v>2186.6646</v>
+      </c>
+      <c r="K136" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="L136" t="n">
+        <v>6</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N136" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O136" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P136" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q136" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R136" t="n">
+        <v>-3.415199999999568</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>FA197B312F42C4A000</t>
+        </is>
+      </c>
+      <c r="T136" t="inlineStr"/>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>FA197B31BE537B2000</t>
+        </is>
+      </c>
+      <c r="V136" t="inlineStr">
+        <is>
+          <t>FA197B31BEACC4A000</t>
+        </is>
+      </c>
+      <c r="W136" t="inlineStr">
+        <is>
+          <t>FA197B315F4704A000</t>
+        </is>
+      </c>
+      <c r="X136" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y136" t="inlineStr">
+        <is>
+          <t>mv :0.03, mv_2m:0.49,  mv_5m : -0.49, mv_30m : -0.42, mv_60m: 8.85</t>
+        </is>
+      </c>
+      <c r="Z136" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="n">
+        <v>0</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>MRNA</t>
+        </is>
+      </c>
+      <c r="D137" s="2" t="n">
+        <v>45553.98063075232</v>
+      </c>
+      <c r="E137" t="n">
+        <v>72.94</v>
+      </c>
+      <c r="F137" t="n">
+        <v>2188.2</v>
+      </c>
+      <c r="G137" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="H137" s="2" t="n">
+        <v>45554.0208669213</v>
+      </c>
+      <c r="I137" t="n">
+        <v>72.97</v>
+      </c>
+      <c r="J137" t="n">
+        <v>2189.1</v>
+      </c>
+      <c r="K137" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="L137" t="n">
+        <v>30</v>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N137" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O137" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P137" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q137" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R137" t="n">
+        <v>0.6500000000000909</v>
+      </c>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>FA197C320F94FB2000</t>
+        </is>
+      </c>
+      <c r="T137" t="inlineStr"/>
+      <c r="U137" t="inlineStr"/>
+      <c r="V137" t="inlineStr"/>
+      <c r="W137" t="inlineStr">
+        <is>
+          <t>FA197C327EDCBB2000</t>
+        </is>
+      </c>
+      <c r="X137" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y137" t="inlineStr">
+        <is>
+          <t>mv :-1.36, mv_2m:-1.62,  mv_5m : 0.75, mv_30m : 3.62, mv_60m: 1.36</t>
+        </is>
+      </c>
+      <c r="Z137" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="n">
+        <v>1</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="D138" s="2" t="n">
+        <v>45553.98121782408</v>
+      </c>
+      <c r="E138" t="n">
+        <v>50.6496</v>
+      </c>
+      <c r="F138" t="n">
+        <v>2177.9328</v>
+      </c>
+      <c r="G138" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H138" s="2" t="n">
+        <v>45554.02390834491</v>
+      </c>
+      <c r="I138" t="n">
+        <v>50.72</v>
+      </c>
+      <c r="J138" t="n">
+        <v>2180.96</v>
+      </c>
+      <c r="K138" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L138" t="n">
+        <v>43</v>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N138" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O138" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P138" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q138" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R138" t="n">
+        <v>2.697199999999993</v>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>FA197C32411CC4A000</t>
+        </is>
+      </c>
+      <c r="T138" t="inlineStr"/>
+      <c r="U138" t="inlineStr">
+        <is>
+          <t>FA197C32F116FB2000</t>
+        </is>
+      </c>
+      <c r="V138" t="inlineStr">
+        <is>
+          <t>FA197C32F1707B2000</t>
+        </is>
+      </c>
+      <c r="W138" t="inlineStr">
+        <is>
+          <t>FA197C327F5E7B2000</t>
+        </is>
+      </c>
+      <c r="X138" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y138" t="inlineStr">
+        <is>
+          <t>mv :-2.42, mv_2m:-2.72,  mv_5m : -0.91, mv_30m : 5.85, mv_60m: 2.54</t>
+        </is>
+      </c>
+      <c r="Z138" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="n">
+        <v>2</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>ETN</t>
+        </is>
+      </c>
+      <c r="D139" s="2" t="n">
+        <v>45553.98130722222</v>
+      </c>
+      <c r="E139" t="n">
+        <v>314.53</v>
+      </c>
+      <c r="F139" t="n">
+        <v>1887.18</v>
+      </c>
+      <c r="G139" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H139" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" t="n">
+        <v>6</v>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N139" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O139" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P139" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R139" t="n">
+        <v>0</v>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>FA197C3248A8FB2000</t>
+        </is>
+      </c>
+      <c r="T139" t="inlineStr"/>
+      <c r="U139" t="inlineStr"/>
+      <c r="V139" t="inlineStr"/>
+      <c r="W139" t="inlineStr"/>
+      <c r="X139" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y139" t="inlineStr">
+        <is>
+          <t>mv :-2.33, mv_2m:-2.63,  mv_5m : -0.54, mv_30m : 6.58, mv_60m: 3.39</t>
+        </is>
+      </c>
+      <c r="Z139" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="n">
+        <v>4</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>SCHW</t>
+        </is>
+      </c>
+      <c r="D140" s="2" t="n">
+        <v>45553.98226488426</v>
+      </c>
+      <c r="E140" t="n">
+        <v>63.98</v>
+      </c>
+      <c r="F140" t="n">
+        <v>2175.32</v>
+      </c>
+      <c r="G140" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H140" s="2" t="n">
+        <v>45554.02270332176</v>
+      </c>
+      <c r="I140" t="n">
+        <v>63.8208</v>
+      </c>
+      <c r="J140" t="n">
+        <v>2169.9072</v>
+      </c>
+      <c r="K140" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="L140" t="n">
+        <v>34</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N140" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O140" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P140" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q140" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R140" t="n">
+        <v>-5.682799999999606</v>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>FA197C32997384A000</t>
+        </is>
+      </c>
+      <c r="T140" t="inlineStr"/>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>FA197C32EFC284A000</t>
+        </is>
+      </c>
+      <c r="V140" t="inlineStr">
+        <is>
+          <t>FA197C32F02DBB2000</t>
+        </is>
+      </c>
+      <c r="W140" t="inlineStr">
+        <is>
+          <t>FA197C32F0B0C4A000</t>
+        </is>
+      </c>
+      <c r="X140" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y140" t="inlineStr">
+        <is>
+          <t>mv :-0.88, mv_2m:1.50,  mv_5m : -0.87, mv_30m : 2.48, mv_60m: 0.73</t>
+        </is>
+      </c>
+      <c r="Z140" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="n">
+        <v>6</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>DXCM</t>
+        </is>
+      </c>
+      <c r="D141" s="2" t="n">
+        <v>45553.98335518518</v>
+      </c>
+      <c r="E141" t="n">
+        <v>70.13</v>
+      </c>
+      <c r="F141" t="n">
+        <v>2174.03</v>
+      </c>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" s="2" t="n">
+        <v>45554.02397006944</v>
+      </c>
+      <c r="I141" t="n">
+        <v>70.02</v>
+      </c>
+      <c r="J141" t="n">
+        <v>2170.62</v>
+      </c>
+      <c r="K141" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="L141" t="n">
+        <v>31</v>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N141" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O141" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P141" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q141" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R141" t="inlineStr"/>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>FA197C32F5847B2000</t>
+        </is>
+      </c>
+      <c r="T141" t="inlineStr"/>
+      <c r="U141" t="inlineStr">
+        <is>
+          <t>FA197C3378EE3B2000</t>
+        </is>
+      </c>
+      <c r="V141" t="inlineStr">
+        <is>
+          <t>FA197C33794C44A000</t>
+        </is>
+      </c>
+      <c r="W141" t="inlineStr">
+        <is>
+          <t>FA197C3379CF84A000</t>
+        </is>
+      </c>
+      <c r="X141" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y141" t="inlineStr">
+        <is>
+          <t>mv :0.21, mv_2m:0.62,  mv_5m : 0.69, mv_30m : 0.79, mv_60m: 0.59</t>
+        </is>
+      </c>
+      <c r="Z141" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="n">
+        <v>7</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>MNST</t>
+        </is>
+      </c>
+      <c r="D142" s="2" t="n">
+        <v>45553.98381877315</v>
+      </c>
+      <c r="E142" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="F142" t="n">
+        <v>2163</v>
+      </c>
+      <c r="G142" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H142" s="2" t="n">
+        <v>45554.02444737269</v>
+      </c>
+      <c r="I142" t="n">
+        <v>51.6304</v>
+      </c>
+      <c r="J142" t="n">
+        <v>2168.4768</v>
+      </c>
+      <c r="K142" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L142" t="n">
+        <v>42</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N142" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O142" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P142" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q142" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R142" t="n">
+        <v>5.146799999999912</v>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>FA197C331C9104A000</t>
+        </is>
+      </c>
+      <c r="T142" t="inlineStr"/>
+      <c r="U142" t="inlineStr">
+        <is>
+          <t>FA197C33775CBB2000</t>
+        </is>
+      </c>
+      <c r="V142" t="inlineStr">
+        <is>
+          <t>FA197C3377CA3B2000</t>
+        </is>
+      </c>
+      <c r="W142" t="inlineStr">
+        <is>
+          <t>FA197C33787FBB2000</t>
+        </is>
+      </c>
+      <c r="X142" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y142" t="inlineStr">
+        <is>
+          <t>mv :3.46, mv_2m:3.87,  mv_5m : 6.40, mv_30m : 9.51, mv_60m: 7.41</t>
+        </is>
+      </c>
+      <c r="Z142" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="n">
+        <v>8</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>NUE</t>
+        </is>
+      </c>
+      <c r="D143" s="2" t="n">
+        <v>45553.98525818287</v>
+      </c>
+      <c r="E143" t="n">
+        <v>143.81</v>
+      </c>
+      <c r="F143" t="n">
+        <v>2157.15</v>
+      </c>
+      <c r="G143" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H143" s="2" t="n">
+        <v>45554.02622417824</v>
+      </c>
+      <c r="I143" t="n">
+        <v>143.64</v>
+      </c>
+      <c r="J143" t="n">
+        <v>2154.6</v>
+      </c>
+      <c r="K143" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="L143" t="n">
+        <v>15</v>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N143" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O143" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P143" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q143" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R143" t="n">
+        <v>-2.720000000000182</v>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>FA197C33960244A000</t>
+        </is>
+      </c>
+      <c r="T143" t="inlineStr"/>
+      <c r="U143" t="inlineStr">
+        <is>
+          <t>FA197C3407C484A000</t>
+        </is>
+      </c>
+      <c r="V143" t="inlineStr">
+        <is>
+          <t>FA197C340813FB2000</t>
+        </is>
+      </c>
+      <c r="W143" t="inlineStr">
+        <is>
+          <t>FA197C34088284A000</t>
+        </is>
+      </c>
+      <c r="X143" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y143" t="inlineStr">
+        <is>
+          <t>mv :2.72, mv_2m:0.89,  mv_5m : 5.89, mv_30m : 8.80, mv_60m: 7.59</t>
+        </is>
+      </c>
+      <c r="Z143" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="n">
+        <v>9</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>MCD</t>
+        </is>
+      </c>
+      <c r="D144" s="2" t="n">
+        <v>45553.98585078704</v>
+      </c>
+      <c r="E144" t="n">
+        <v>294.63</v>
+      </c>
+      <c r="F144" t="n">
+        <v>2062.41</v>
+      </c>
+      <c r="G144" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H144" s="2" t="n">
+        <v>45554.02868767361</v>
+      </c>
+      <c r="I144" t="n">
+        <v>294.51</v>
+      </c>
+      <c r="J144" t="n">
+        <v>2061.57</v>
+      </c>
+      <c r="K144" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L144" t="n">
+        <v>7</v>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N144" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O144" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P144" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q144" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R144" t="n">
+        <v>-0.9600000000001455</v>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>FA197C33C8023B2000</t>
+        </is>
+      </c>
+      <c r="T144" t="inlineStr"/>
+      <c r="U144" t="inlineStr">
+        <is>
+          <t>FA197C349348FB2000</t>
+        </is>
+      </c>
+      <c r="V144" t="inlineStr">
+        <is>
+          <t>FA197C3493A284A000</t>
+        </is>
+      </c>
+      <c r="W144" t="inlineStr">
+        <is>
+          <t>FA197C3494237B2000</t>
+        </is>
+      </c>
+      <c r="X144" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y144" t="inlineStr">
+        <is>
+          <t>mv :4.97, mv_2m:3.46,  mv_5m : 10.47, mv_30m : 18.47, mv_60m: 16.65</t>
+        </is>
+      </c>
+      <c r="Z144" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>10</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>CVX</t>
+        </is>
+      </c>
+      <c r="D145" s="2" t="n">
+        <v>45553.98596554398</v>
+      </c>
+      <c r="E145" t="n">
+        <v>144.14</v>
+      </c>
+      <c r="F145" t="n">
+        <v>2162.1</v>
+      </c>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" s="2" t="n">
+        <v>45554.03215778935</v>
+      </c>
+      <c r="I145" t="n">
+        <v>144.05</v>
+      </c>
+      <c r="J145" t="n">
+        <v>2160.75</v>
+      </c>
+      <c r="K145" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="L145" t="n">
+        <v>15</v>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N145" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O145" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P145" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q145" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R145" t="inlineStr"/>
+      <c r="S145" t="inlineStr">
+        <is>
+          <t>FA197C33D1B204A000</t>
+        </is>
+      </c>
+      <c r="T145" t="inlineStr"/>
+      <c r="U145" t="inlineStr">
+        <is>
+          <t>FA197C3494813B2000</t>
+        </is>
+      </c>
+      <c r="V145" t="inlineStr">
+        <is>
+          <t>FA197C3494E57B2000</t>
+        </is>
+      </c>
+      <c r="W145" t="inlineStr">
+        <is>
+          <t>FA197C34956A44A000</t>
+        </is>
+      </c>
+      <c r="X145" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y145" t="inlineStr">
+        <is>
+          <t>mv :5.74, mv_2m:4.22,  mv_5m : 10.77, mv_30m : 18.80, mv_60m: 17.40</t>
+        </is>
+      </c>
+      <c r="Z145" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="n">
+        <v>14</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>USB</t>
+        </is>
+      </c>
+      <c r="D146" s="2" t="n">
+        <v>45553.9873989699</v>
+      </c>
+      <c r="E146" t="n">
+        <v>44.94</v>
+      </c>
+      <c r="F146" t="n">
+        <v>2157.12</v>
+      </c>
+      <c r="G146" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H146" s="2" t="n">
+        <v>45554.02877569445</v>
+      </c>
+      <c r="I146" t="n">
+        <v>45.0405</v>
+      </c>
+      <c r="J146" t="n">
+        <v>2161.944</v>
+      </c>
+      <c r="K146" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="L146" t="n">
+        <v>48</v>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N146" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O146" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P146" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q146" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R146" t="n">
+        <v>4.464000000000069</v>
+      </c>
+      <c r="S146" t="inlineStr">
+        <is>
+          <t>FA197C344AA4FB2000</t>
+        </is>
+      </c>
+      <c r="T146" t="inlineStr"/>
+      <c r="U146" t="inlineStr">
+        <is>
+          <t>FA197C350FC23B2000</t>
+        </is>
+      </c>
+      <c r="V146" t="inlineStr">
+        <is>
+          <t>FA197C35101B04A000</t>
+        </is>
+      </c>
+      <c r="W146" t="inlineStr">
+        <is>
+          <t>FA197C34ABD67B2000</t>
+        </is>
+      </c>
+      <c r="X146" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y146" t="inlineStr">
+        <is>
+          <t>mv :6.84, mv_2m:1.56,  mv_5m : 8.82, mv_30m : 21.60, mv_60m: 19.40</t>
+        </is>
+      </c>
+      <c r="Z146" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="n">
+        <v>17</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="D147" s="2" t="n">
+        <v>45553.98995776621</v>
+      </c>
+      <c r="E147" t="n">
+        <v>298.03</v>
+      </c>
+      <c r="F147" t="n">
+        <v>2086.21</v>
+      </c>
+      <c r="G147" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H147" s="2" t="n">
+        <v>45554.03060295139</v>
+      </c>
+      <c r="I147" t="n">
+        <v>297.4986</v>
+      </c>
+      <c r="J147" t="n">
+        <v>2082.4902</v>
+      </c>
+      <c r="K147" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L147" t="n">
+        <v>7</v>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N147" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O147" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P147" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q147" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R147" t="n">
+        <v>-3.82979999999985</v>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>FA197C35228B3B2000</t>
+        </is>
+      </c>
+      <c r="T147" t="inlineStr"/>
+      <c r="U147" t="inlineStr">
+        <is>
+          <t>FA197C359939FB2000</t>
+        </is>
+      </c>
+      <c r="V147" t="inlineStr">
+        <is>
+          <t>FA197C35999C7B2000</t>
+        </is>
+      </c>
+      <c r="W147" t="inlineStr">
+        <is>
+          <t>FA197C359A1D3B2000</t>
+        </is>
+      </c>
+      <c r="X147" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y147" t="inlineStr">
+        <is>
+          <t>mv :6.08, mv_2m:0.28,  mv_5m : 1.29, mv_30m : 10.40, mv_60m: 8.25</t>
+        </is>
+      </c>
+      <c r="Z147" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="n">
+        <v>18</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>OXY</t>
+        </is>
+      </c>
+      <c r="D148" s="2" t="n">
+        <v>45553.99044223379</v>
+      </c>
+      <c r="E148" t="n">
+        <v>52.1</v>
+      </c>
+      <c r="F148" t="n">
+        <v>2188.2</v>
+      </c>
+      <c r="G148" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H148" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" t="n">
+        <v>42</v>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>cancelled</t>
+        </is>
+      </c>
+      <c r="N148" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O148" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P148" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q148" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R148" t="n">
+        <v>0</v>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>FA197C354B68BB2000</t>
+        </is>
+      </c>
+      <c r="T148" t="inlineStr"/>
+      <c r="U148" t="inlineStr"/>
+      <c r="V148" t="inlineStr"/>
+      <c r="W148" t="inlineStr"/>
+      <c r="X148" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y148" t="inlineStr">
+        <is>
+          <t>mv :5.57, mv_2m:-0.24,  mv_5m : -0.94, mv_30m : 17.26, mv_60m: 13.14</t>
+        </is>
+      </c>
+      <c r="Z148" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="n">
+        <v>20</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>CHTR</t>
+        </is>
+      </c>
+      <c r="D149" s="2" t="n">
+        <v>45553.99209734954</v>
+      </c>
+      <c r="E149" t="n">
+        <v>342.38</v>
+      </c>
+      <c r="F149" t="n">
+        <v>2054.28</v>
+      </c>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" s="2" t="n">
+        <v>45554.03220837963</v>
+      </c>
+      <c r="I149" t="n">
+        <v>341.36</v>
+      </c>
+      <c r="J149" t="n">
+        <v>2048.16</v>
+      </c>
+      <c r="K149" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L149" t="n">
+        <v>6</v>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N149" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O149" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P149" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q149" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R149" t="inlineStr"/>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>FA197C35D71104A000</t>
+        </is>
+      </c>
+      <c r="T149" t="inlineStr"/>
+      <c r="U149" t="inlineStr">
+        <is>
+          <t>FA197C3624A8FB2000</t>
+        </is>
+      </c>
+      <c r="V149" t="inlineStr">
+        <is>
+          <t>FA197C362512BB2000</t>
+        </is>
+      </c>
+      <c r="W149" t="inlineStr">
+        <is>
+          <t>FA197C36258E84A000</t>
+        </is>
+      </c>
+      <c r="X149" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y149" t="inlineStr">
+        <is>
+          <t>mv :3.98, mv_2m:-0.92,  mv_5m : -2.98, mv_30m : 12.56, mv_60m: 9.95</t>
+        </is>
+      </c>
+      <c r="Z149" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>21</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>ETN</t>
+        </is>
+      </c>
+      <c r="D150" s="2" t="n">
+        <v>45553.99265765047</v>
+      </c>
+      <c r="E150" t="n">
+        <v>317.7</v>
+      </c>
+      <c r="F150" t="n">
+        <v>1906.2</v>
+      </c>
+      <c r="G150" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H150" s="2" t="n">
+        <v>45554.03282503472</v>
+      </c>
+      <c r="I150" t="n">
+        <v>316.41</v>
+      </c>
+      <c r="J150" t="n">
+        <v>1898.46</v>
+      </c>
+      <c r="K150" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="L150" t="n">
+        <v>6</v>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="N150" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O150" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P150" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q150" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R150" t="n">
+        <v>-7.840000000000009</v>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>FA197C36065784A000</t>
+        </is>
+      </c>
+      <c r="T150" t="inlineStr"/>
+      <c r="U150" t="inlineStr"/>
+      <c r="V150" t="inlineStr"/>
+      <c r="W150" t="inlineStr">
+        <is>
+          <t>FA197C363B1844A000</t>
+        </is>
+      </c>
+      <c r="X150" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y150" t="inlineStr">
+        <is>
+          <t>mv :3.63, mv_2m:-1.23,  mv_5m : -4.67, mv_30m : 12.79, mv_60m: 11.04</t>
+        </is>
+      </c>
+      <c r="Z150" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>CMCSA</t>
+        </is>
+      </c>
+      <c r="D151" s="2" t="n">
+        <v>45553.99833571322</v>
+      </c>
+      <c r="E151" t="n">
+        <v>39.59</v>
+      </c>
+      <c r="F151" t="n">
+        <v>2177.45</v>
+      </c>
+      <c r="G151" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H151" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" t="n">
+        <v>55</v>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>placed</t>
+        </is>
+      </c>
+      <c r="N151" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O151" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P151" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q151" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R151" t="n">
+        <v>0</v>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>FA197C37E56CBB2000</t>
+        </is>
+      </c>
+      <c r="T151" t="inlineStr"/>
+      <c r="U151" t="inlineStr"/>
+      <c r="V151" t="inlineStr"/>
+      <c r="W151" t="inlineStr"/>
+      <c r="X151" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y151" t="inlineStr">
+        <is>
+          <t>mv :-4.61, mv_2m:-1.67,  mv_5m : -5.33, mv_30m : 4.19, mv_60m: 10.45</t>
+        </is>
+      </c>
+      <c r="Z151" t="inlineStr">
+        <is>
+          <t>E. Australia Standard Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="n">
+        <v>1</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>CVS</t>
+        </is>
+      </c>
+      <c r="D152" s="2" t="n">
+        <v>45553.99891814552</v>
+      </c>
+      <c r="E152" t="n">
+        <v>58.14</v>
+      </c>
+      <c r="F152" t="n">
+        <v>2151.18</v>
+      </c>
+      <c r="G152" t="n">
+        <v>1.111</v>
+      </c>
+      <c r="H152" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="n">
+        <v>0</v>
+      </c>
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" t="n">
+        <v>37</v>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>placed</t>
+        </is>
+      </c>
+      <c r="N152" t="n">
+        <v>1.005</v>
+      </c>
+      <c r="O152" t="n">
+        <v>0.995</v>
+      </c>
+      <c r="P152" t="n">
+        <v>1.006</v>
+      </c>
+      <c r="Q152" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="R152" t="n">
+        <v>0</v>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>FA197C381691C4A000</t>
+        </is>
+      </c>
+      <c r="T152" t="inlineStr"/>
+      <c r="U152" t="inlineStr"/>
+      <c r="V152" t="inlineStr"/>
+      <c r="W152" t="inlineStr"/>
+      <c r="X152" t="inlineStr">
+        <is>
+          <t>1h</t>
+        </is>
+      </c>
+      <c r="Y152" t="inlineStr">
+        <is>
+          <t>mv :-4.67, mv_2m:0.24,  mv_5m : 0.38, mv_30m : 1.14, mv_60m: 1.32</t>
+        </is>
+      </c>
+      <c r="Z152" t="inlineStr">
         <is>
           <t>E. Australia Standard Time</t>
         </is>

</xml_diff>